<commit_message>
Update task backlog and test script documents
Revised Codex task backlog spreadsheet and Phase 1 & 2 test script document to reflect latest project changes and requirements.
</commit_message>
<xml_diff>
--- a/Docs/Codex_Task_Backlog-20251202.xlsx
+++ b/Docs/Codex_Task_Backlog-20251202.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\GitHub\LalaLaunchPlugin\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Github\LalaLaunchPlugin\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAAF4562-8F6F-44CC-82DA-AC1AC5922932}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDF36C50-59AD-42EC-B3A9-593D130A7038}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="30" windowWidth="28770" windowHeight="15450" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28890" yWindow="555" windowWidth="28005" windowHeight="14790" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tasking Order" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="188">
   <si>
     <t>ID</t>
   </si>
@@ -572,10 +572,6 @@
 Added a comprehensive live snapshot reset that clears lap pace, leader delta, fuel averages, and confidence so new car/track combinations start from profile defaults or empty live data  https://github.com/Lalabot77/LalaLaunchPlugin/pull/137</t>
   </si>
   <si>
-    <t>Updated the extra-time-after-zero helper to use a continuous decimal-lap calculation based on leader and driver lap times, ensuring smoother “Est. Drive Time After Timer Zero” updates with pace slider changes.
-https://github.com/Lalabot77/LalaLaunchPlugin/pull/139</t>
-  </si>
-  <si>
     <t>Added leader pace delta tracking with helper updates and resets so SimHub never surfaces stale leader pace data when averages change or telemetry is unavailable.
 Exposed new SimHub parameters for leader average lap time and leader-versus-player delta alongside existing pace metrics.
 https://github.com/Lalabot77/LalaLaunchPlugin/pull/140</t>
@@ -633,6 +629,128 @@
 Tracked seed presence, fresh sample counts, and fallback flags while resetting models on session transitions to ensure seeded race starts begin with controlled confidence that grows with clean laps.
 Detected car/track changes to clear stored seeds and confidence immediately, preventing stale values from surfacing in the Fuel tab or SimHub outputs.
 https://github.com/Lalabot77/LalaLaunchPlugin/pull/146</t>
+  </si>
+  <si>
+    <t>Updated the extra-time-after-zero helper to use a continuous decimal-lap calculation based on leader and driver lap times, ensuring smoother “Est. Drive Time After Timer Zero” updates with pace slider changes.
+https://github.com/Lalabot77/LalaLaunchPlugin/pull/139
+2nd pass:
+Finish-timing logging is gated by one-shot latches: the leader’s checkered time records only on the first checkered tick (LeaderHasFinished), and the combined leader/driver message is emitted only when the driver next completes a lap under checkered before the state resets, avoiding per-tick spam.
+ResetFinishTimingState clears both the logging latches and LeaderHasFinished, and it’s invoked on plugin startup and whenever the session changes or the session type is not a race, ensuring clean initialization and per-session resets as requested
+https://github.com/Lalabot77/LalaLaunchPlugin/pull/148</t>
+  </si>
+  <si>
+    <t>LALA-039: Fix the Avg Lap textbox on the Fuel tab so that it correctly tracks the planning source (Profile vs Live Snapshot), while still allowing a manual override that is reset when the source is changed. Right now, SelectedPlanningSourceMode only passes applyLapTime: false into ApplyPlanningSourceToAutoFields, so flipping between Profile and Live only affects Fuel Per Lap and leaves the Avg Lap textbox stuck on whatever it had before. In addition, IsEstimatedLapTimeManual is not cleared when the user changes planning source, so a manual entry can block future auto updates. Update FuelCalcs so that: (1) when SelectedPlanningSourceMode is changed, both LapTime and Fuel Per Lap are refreshed from the chosen source if they are not manual, and manual lap time is explicitly dropped when changing the planning source (i.e. clear IsEstimatedLapTimeManual and then call ApplyPlanningSourceToAutoFields with applyLapTime: true, applyFuel: true); (2) switching to Profile mode with profile averages available immediately populates the Avg Lap textbox with the profile dry/wet average and sets LapTimeSourceInfo to a “Profile avg” label; (3) switching to LiveSnapshot mode when a valid _liveAvgLapSeconds is available immediately populates the Avg Lap textbox from GetLiveAverageLapTimeSnapshot and sets LapTimeSourceInfo to “Live avg”; (4) manual edits to the Avg Lap textbox still work by setting IsEstimatedLapTimeManual = true and tagging the source as “Manual (user entry)”, but the next change of SelectedPlanningSourceMode must override that manual state and re-sync to the newly chosen source; and (5) when planning source is LiveSnapshot and IsEstimatedLapTimeManual is false, updates to _liveAvgLapSeconds should be reflected in the Avg Lap textbox in near-real time (e.g. by calling ApplyPlanningSourceToAutoFields(applyLapTime: true, applyFuel: false) or equivalent whenever the live average is updated). After this change, toggling Profile/Live always reloads the Avg Lap textbox from the respective source when data is available, manual override is possible but clearly overridden by a source toggle, and the Live planning source keeps the Avg Lap textbox in sync with the evolving live average.</t>
+  </si>
+  <si>
+    <t>Clearing manual lap-time overrides when the planning source changes now refreshes both lap time and fuel from the newly selected source.
+Live average lap-time updates in Live Snapshot mode now feed the Avg Lap textbox in real time while respecting manual overrides.
+https://github.com/Lalabot77/LalaLaunchPlugin/pull/147</t>
+  </si>
+  <si>
+    <t>LALA-40</t>
+  </si>
+  <si>
+    <t>Auto Save some data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Some data should be auto saved when it is good data. Avg Lap and count dry and wet, eco, avg and max fuel burn and counts. </t>
+  </si>
+  <si>
+    <t>LALA-41</t>
+  </si>
+  <si>
+    <t>LALA-42</t>
+  </si>
+  <si>
+    <t>LALA-43</t>
+  </si>
+  <si>
+    <t>LALA-44</t>
+  </si>
+  <si>
+    <t>LALA-45</t>
+  </si>
+  <si>
+    <t>LALA-46</t>
+  </si>
+  <si>
+    <t>LALA-47</t>
+  </si>
+  <si>
+    <t>LALA-48</t>
+  </si>
+  <si>
+    <t>LALA-49</t>
+  </si>
+  <si>
+    <t>LALA-50</t>
+  </si>
+  <si>
+    <t>Fuel Planner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avg Lap time needs a helper button to reset to live or profile (which ever is in use). </t>
+  </si>
+  <si>
+    <t>This can follow the style of the reset to live feature for the Pace vs Leader section</t>
+  </si>
+  <si>
+    <t>UI</t>
+  </si>
+  <si>
+    <t>Track Condition info terxt to be moved right in line with radio buttons</t>
+  </si>
+  <si>
+    <t>Track Condition info text move</t>
+  </si>
+  <si>
+    <t>Fuel Calcs</t>
+  </si>
+  <si>
+    <t>Pace vs Leader Negative Values</t>
+  </si>
+  <si>
+    <t>It shouild not be possible to have a negative leader delta value and when lapped the system still needs to produce the correct delta</t>
+  </si>
+  <si>
+    <t>Values can be negative when lapped by leader or when lapping faster</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Profiles  </t>
+  </si>
+  <si>
+    <t>Race Pace Delta Saving</t>
+  </si>
+  <si>
+    <t>The race pace delta is in Profiles sub tab Fuel but should be moved to Tracks where it can be saved with other parameters. A valid figure can be saved once enough samples are gathered</t>
+  </si>
+  <si>
+    <t>Live Fuel</t>
+  </si>
+  <si>
+    <t>Delta After Stop Handling</t>
+  </si>
+  <si>
+    <t>Need to tie this to the selections the driver has made. If Refuel is selected, Auto Fuel, amount to be put in tank, amount that will actually fit etc..</t>
+  </si>
+  <si>
+    <t>Delta After Stop shows true situation</t>
+  </si>
+  <si>
+    <t>Modified Helper needs to list what changed "Modified: Avg Lap time, Pit Loss…"</t>
+  </si>
+  <si>
+    <t>Planner</t>
+  </si>
+  <si>
+    <t>Stale Avg Burn Value</t>
+  </si>
+  <si>
+    <t>The Avg Burn value for ther first track in the list for the selected car is persisting across sessions</t>
+  </si>
+  <si>
+    <t>This is not functioning well. Need to log exactly what it does.
+Refresh in profile view resets car and track to default</t>
   </si>
 </sst>
 </file>
@@ -670,12 +788,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -705,12 +829,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1211,13 +1338,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M20"/>
+  <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E13" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="F8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H14" sqref="H14"/>
+      <selection pane="bottomRight" activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1401,7 +1528,10 @@
         <v>129</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>183</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>89</v>
@@ -1526,7 +1656,10 @@
         <v>135</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="240" x14ac:dyDescent="0.25">
@@ -1555,7 +1688,7 @@
         <v>65</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="345" x14ac:dyDescent="0.25">
@@ -1584,7 +1717,7 @@
         <v>74</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="255" x14ac:dyDescent="0.25">
@@ -1613,7 +1746,7 @@
         <v>77</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="300" x14ac:dyDescent="0.25">
@@ -1642,7 +1775,7 @@
         <v>80</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="375" x14ac:dyDescent="0.25">
@@ -1671,7 +1804,7 @@
         <v>83</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="360" x14ac:dyDescent="0.25">
@@ -1755,7 +1888,7 @@
         <v>112</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>138</v>
+        <v>150</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
@@ -1784,7 +1917,7 @@
         <v>116</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="300" x14ac:dyDescent="0.25">
@@ -1816,9 +1949,9 @@
         <v>137</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>88</v>
@@ -1827,16 +1960,167 @@
         <v>67</v>
       </c>
       <c r="D20" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>148</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>149</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>58</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>165</v>
       </c>
     </row>
   </sheetData>

</xml_diff>